<commit_message>
Update the column width
</commit_message>
<xml_diff>
--- a/physics/README.xlsx
+++ b/physics/README.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25516"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20910"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="-460" windowWidth="28800" windowHeight="18000" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="37460" windowHeight="21140" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="LaTeX" sheetId="1" r:id="rId1"/>
@@ -1601,20 +1601,32 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:T123"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="115" zoomScaleNormal="115" zoomScalePageLayoutView="115" workbookViewId="0">
-      <selection activeCell="M7" sqref="M7"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" zoomScalePageLayoutView="115" workbookViewId="0">
+      <selection activeCell="I9" sqref="I9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
-    <col min="12" max="12" width="10.83203125" style="4"/>
-    <col min="13" max="13" width="7.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="2.1640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="3.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.83203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="19.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="6.1640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="3.33203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="2.1640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="1.83203125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="12.83203125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="6.1640625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="1.83203125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="2.1640625" style="4" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="10.5" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="4.33203125" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="30.83203125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="35.5" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="2.6640625" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="1.6640625" bestFit="1" customWidth="1"/>
     <col min="18" max="18" width="13.5" bestFit="1" customWidth="1"/>
     <col min="19" max="19" width="1.83203125" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="1.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:20">

</xml_diff>